<commit_message>
AIP-1584 AIP-1586 Updated test data for some of the cablings
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_16Channel/1U1U3I3I3I.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_16Channel/1U1U3I3I3I.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51526F86-808C-4EF8-AC43-6EE5A56FE4F1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D79B5CA-BFC1-464A-A687-12AEC3620BDE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeviceInfo" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="128">
   <si>
     <t>Channel</t>
   </si>
@@ -185,12 +185,6 @@
     <t>Channel[15]</t>
   </si>
   <si>
-    <t>Channel[16]</t>
-  </si>
-  <si>
-    <t>Channel[17]</t>
-  </si>
-  <si>
     <t>UNIT</t>
   </si>
   <si>
@@ -257,12 +251,6 @@
     <t>CalibrationFileName</t>
   </si>
   <si>
-    <t>10.75.58.51</t>
-  </si>
-  <si>
-    <t>sn409026540_6U_12I.cal</t>
-  </si>
-  <si>
     <t>Channel_Number_DSP1</t>
   </si>
   <si>
@@ -414,6 +402,12 @@
   </si>
   <si>
     <t>DSP_2_Feeder_Map_2</t>
+  </si>
+  <si>
+    <t>10.75.58.66</t>
+  </si>
+  <si>
+    <t>6U_10I.cal</t>
   </si>
 </sst>
 </file>
@@ -737,7 +731,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,18 +742,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -773,7 +767,7 @@
   <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:J13"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,13 +815,13 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" t="s">
         <v>57</v>
-      </c>
-      <c r="K1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -841,7 +835,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -859,13 +853,13 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -879,13 +873,13 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
         <v>18</v>
@@ -897,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -911,13 +905,13 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
@@ -929,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -943,7 +937,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -961,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -975,7 +969,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
@@ -993,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W6" t="s">
         <v>19</v>
@@ -1011,7 +1005,7 @@
         <v>15</v>
       </c>
       <c r="AB6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -1025,7 +1019,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
@@ -1043,7 +1037,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W7" t="s">
         <v>20</v>
@@ -1055,13 +1049,13 @@
         <v>11</v>
       </c>
       <c r="Z7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AA7" t="s">
         <v>16</v>
       </c>
       <c r="AB7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -1075,7 +1069,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1093,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W8" t="s">
         <v>21</v>
@@ -1102,13 +1096,13 @@
         <v>12</v>
       </c>
       <c r="Z8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AA8" t="s">
         <v>17</v>
       </c>
       <c r="AB8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -1122,7 +1116,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -1140,22 +1134,22 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W9" t="s">
         <v>22</v>
       </c>
       <c r="Y9" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA9" t="s">
         <v>68</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AB9" t="s">
         <v>69</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -1169,7 +1163,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -1187,22 +1181,22 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W10" t="s">
         <v>23</v>
       </c>
       <c r="Y10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Z10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AA10" t="s">
         <v>18</v>
       </c>
       <c r="AB10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -1216,13 +1210,13 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G11" t="s">
         <v>15</v>
@@ -1234,13 +1228,13 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W11" t="s">
         <v>24</v>
       </c>
       <c r="Y11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -1254,13 +1248,13 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
         <v>18</v>
@@ -1272,7 +1266,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W12" t="s">
         <v>25</v>
@@ -1289,13 +1283,13 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G13" t="s">
         <v>18</v>
@@ -1307,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W13" t="s">
         <v>26</v>
@@ -1324,13 +1318,13 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G14" t="s">
         <v>15</v>
@@ -1342,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W14" t="s">
         <v>27</v>
@@ -1359,13 +1353,13 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G15" t="s">
         <v>16</v>
@@ -1377,7 +1371,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W15" t="s">
         <v>28</v>
@@ -1394,13 +1388,13 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G16" t="s">
         <v>17</v>
@@ -1412,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W16" t="s">
         <v>29</v>
@@ -1429,13 +1423,13 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
         <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G17" t="s">
         <v>18</v>
@@ -1447,78 +1441,18 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18" t="s">
-        <v>71</v>
-      </c>
       <c r="W18" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-      <c r="J19" t="s">
-        <v>71</v>
-      </c>
       <c r="W19" t="s">
         <v>32</v>
       </c>
@@ -1545,22 +1479,22 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C19" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C17" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$X$6:$X$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E19" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E17" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$Y$6:$Y$11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F19" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F17" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>$Z$6:$Z$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G19" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G17" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>$AA$6:$AA$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J19" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J17" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>$AB$6:$AB$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B20" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B18" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>$W$6:$W$23</formula1>
     </dataValidation>
   </dataValidations>
@@ -1575,22 +1509,22 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -1598,7 +1532,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -1606,7 +1540,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -1614,7 +1548,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
@@ -1622,7 +1556,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -1630,7 +1564,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B7" s="2">
         <v>-1</v>
@@ -1646,8 +1580,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,15 +1591,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1673,7 +1607,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -1681,7 +1615,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -1689,7 +1623,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -1697,7 +1631,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
@@ -1705,7 +1639,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B7" s="1">
         <v>10</v>
@@ -1713,7 +1647,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -1721,7 +1655,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -1729,7 +1663,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1737,7 +1671,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B11" s="1">
         <v>3</v>
@@ -1745,7 +1679,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B12" s="1">
         <v>4</v>
@@ -1753,7 +1687,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B13" s="1">
         <v>5</v>
@@ -1761,7 +1695,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B14" s="1">
         <v>6</v>
@@ -1769,7 +1703,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -1777,7 +1711,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B16" s="1">
         <v>3</v>
@@ -1785,7 +1719,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1793,7 +1727,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B18">
         <v>7</v>
@@ -1801,7 +1735,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B19">
         <v>8</v>
@@ -1809,7 +1743,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B20">
         <v>9</v>
@@ -1817,7 +1751,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1825,7 +1759,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -1833,7 +1767,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1841,7 +1775,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B24">
         <v>13</v>
@@ -1849,7 +1783,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B25">
         <v>14</v>
@@ -1857,7 +1791,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B26">
         <v>15</v>
@@ -1865,7 +1799,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1873,7 +1807,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -1881,7 +1815,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -1889,7 +1823,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -1897,7 +1831,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -1905,7 +1839,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B32">
         <v>11</v>
@@ -1913,7 +1847,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -1921,7 +1855,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -1929,7 +1863,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1937,7 +1871,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B36">
         <v>12</v>
@@ -1945,23 +1879,23 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B37">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B38">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1969,15 +1903,15 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1993,8 +1927,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2007,16 +1941,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2128,7 +2062,7 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2142,7 +2076,7 @@
         <v>8</v>
       </c>
       <c r="D10">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>